<commit_message>
NullPointerException bug in validateStudent() fixed
</commit_message>
<xml_diff>
--- a/src/main/resources/universityInfo.xlsx
+++ b/src/main/resources/universityInfo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\25_exercise_25.9\Project_24-7\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergey\Documents\Java\31_exercise_26.9\Project_24-7\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99AA635B-AD37-4649-84A5-2F4E82FE07E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B0F30A9-BEA8-4F50-B3E8-2310A0A3DF5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="1575" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Студенты" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="41">
   <si>
     <t>id университета</t>
   </si>
@@ -84,18 +84,12 @@
     <t>МПИ</t>
   </si>
   <si>
-    <t>Московский Государственный Медицинский Университет</t>
-  </si>
-  <si>
     <t>МГМУ</t>
   </si>
   <si>
     <t>Тамбовский Университет Медицины</t>
   </si>
   <si>
-    <t>ТУМ</t>
-  </si>
-  <si>
     <t>Самарский Медицинский Институт</t>
   </si>
   <si>
@@ -141,12 +135,6 @@
     <t>Сидоров Е. Г.</t>
   </si>
   <si>
-    <t>Витальев В. А.</t>
-  </si>
-  <si>
-    <t>Петров П. А.</t>
-  </si>
-  <si>
     <t>Алексеев С. В.</t>
   </si>
   <si>
@@ -154,6 +142,9 @@
   </si>
   <si>
     <t>Васильев В. П.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     </t>
   </si>
 </sst>
 </file>
@@ -199,10 +190,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -543,8 +535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,13 +549,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -571,7 +563,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C2" s="2">
         <v>2</v>
@@ -585,7 +577,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C3" s="2">
         <v>2</v>
@@ -599,7 +591,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C4" s="2">
         <v>3</v>
@@ -613,7 +605,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C5" s="2">
         <v>4</v>
@@ -627,7 +619,7 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
@@ -641,7 +633,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C7" s="2">
         <v>2</v>
@@ -654,9 +646,6 @@
       <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="B8" t="s">
-        <v>39</v>
-      </c>
       <c r="C8" s="2">
         <v>2</v>
       </c>
@@ -668,7 +657,7 @@
       <c r="A9" t="s">
         <v>5</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>40</v>
       </c>
       <c r="C9" s="2">
@@ -683,7 +672,7 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C10" s="2">
         <v>1</v>
@@ -697,7 +686,7 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C11" s="2">
         <v>3</v>
@@ -711,7 +700,7 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C12" s="2">
         <v>4</v>
@@ -730,8 +719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -798,11 +787,8 @@
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
       </c>
       <c r="D4">
         <v>1960</v>
@@ -816,10 +802,10 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" t="s">
-        <v>23</v>
+        <v>21</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="D5">
         <v>1995</v>
@@ -833,10 +819,10 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D6">
         <v>1936</v>
@@ -850,10 +836,10 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D7">
         <v>2003</v>
@@ -867,10 +853,10 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D8">
         <v>1989</v>

</xml_diff>

<commit_message>
universityInfo.xlsx moved to resources
</commit_message>
<xml_diff>
--- a/src/main/resources/universityInfo.xlsx
+++ b/src/main/resources/universityInfo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergey\Documents\Java\31_exercise_26.9\Project_24-7\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\25_exercise_25.9\Project_24-7\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B0F30A9-BEA8-4F50-B3E8-2310A0A3DF5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99AA635B-AD37-4649-84A5-2F4E82FE07E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="1575" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Студенты" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="44">
   <si>
     <t>id университета</t>
   </si>
@@ -84,12 +84,18 @@
     <t>МПИ</t>
   </si>
   <si>
+    <t>Московский Государственный Медицинский Университет</t>
+  </si>
+  <si>
     <t>МГМУ</t>
   </si>
   <si>
     <t>Тамбовский Университет Медицины</t>
   </si>
   <si>
+    <t>ТУМ</t>
+  </si>
+  <si>
     <t>Самарский Медицинский Институт</t>
   </si>
   <si>
@@ -135,6 +141,12 @@
     <t>Сидоров Е. Г.</t>
   </si>
   <si>
+    <t>Витальев В. А.</t>
+  </si>
+  <si>
+    <t>Петров П. А.</t>
+  </si>
+  <si>
     <t>Алексеев С. В.</t>
   </si>
   <si>
@@ -142,9 +154,6 @@
   </si>
   <si>
     <t>Васильев В. П.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     </t>
   </si>
 </sst>
 </file>
@@ -190,11 +199,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -535,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,13 +557,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -563,7 +571,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C2" s="2">
         <v>2</v>
@@ -577,7 +585,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C3" s="2">
         <v>2</v>
@@ -591,7 +599,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C4" s="2">
         <v>3</v>
@@ -605,7 +613,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C5" s="2">
         <v>4</v>
@@ -619,7 +627,7 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
@@ -633,7 +641,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C7" s="2">
         <v>2</v>
@@ -646,6 +654,9 @@
       <c r="A8" t="s">
         <v>5</v>
       </c>
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
       <c r="C8" s="2">
         <v>2</v>
       </c>
@@ -657,7 +668,7 @@
       <c r="A9" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" t="s">
         <v>40</v>
       </c>
       <c r="C9" s="2">
@@ -672,7 +683,7 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C10" s="2">
         <v>1</v>
@@ -686,7 +697,7 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C11" s="2">
         <v>3</v>
@@ -700,7 +711,7 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C12" s="2">
         <v>4</v>
@@ -719,8 +730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -787,8 +798,11 @@
       <c r="A4" t="s">
         <v>7</v>
       </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D4">
         <v>1960</v>
@@ -802,10 +816,10 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>40</v>
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
       </c>
       <c r="D5">
         <v>1995</v>
@@ -819,10 +833,10 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D6">
         <v>1936</v>
@@ -836,10 +850,10 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D7">
         <v>2003</v>
@@ -853,10 +867,10 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D8">
         <v>1989</v>

</xml_diff>

<commit_message>
added JAXB export to file
</commit_message>
<xml_diff>
--- a/src/main/resources/universityInfo.xlsx
+++ b/src/main/resources/universityInfo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergey\IdeaProjects\39_exersize_27.8\Project_24-7\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\25_exercise_25.9\Project_24-7\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1065EEC-5F3B-4598-A060-91E5042C4F3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99AA635B-AD37-4649-84A5-2F4E82FE07E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="1575" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Студенты" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="44">
   <si>
     <t>id университета</t>
   </si>
@@ -93,6 +93,9 @@
     <t>Тамбовский Университет Медицины</t>
   </si>
   <si>
+    <t>ТУМ</t>
+  </si>
+  <si>
     <t>Самарский Медицинский Институт</t>
   </si>
   <si>
@@ -133,6 +136,9 @@
   </si>
   <si>
     <t>Соколов В. В.</t>
+  </si>
+  <si>
+    <t>Сидоров Е. Г.</t>
   </si>
   <si>
     <t>Витальев В. А.</t>
@@ -193,11 +199,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -538,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,13 +557,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -566,7 +571,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C2" s="2">
         <v>2</v>
@@ -580,7 +585,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C3" s="2">
         <v>2</v>
@@ -594,7 +599,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C4" s="2">
         <v>3</v>
@@ -608,7 +613,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C5" s="2">
         <v>4</v>
@@ -622,7 +627,7 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
@@ -635,6 +640,9 @@
       <c r="A7" t="s">
         <v>8</v>
       </c>
+      <c r="B7" t="s">
+        <v>38</v>
+      </c>
       <c r="C7" s="2">
         <v>2</v>
       </c>
@@ -647,10 +655,10 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="3">
-        <v>0.02</v>
+        <v>39</v>
+      </c>
+      <c r="C8" s="2">
+        <v>2</v>
       </c>
       <c r="D8" s="2">
         <v>4</v>
@@ -661,7 +669,7 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C9" s="2">
         <v>1</v>
@@ -675,7 +683,7 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C10" s="2">
         <v>1</v>
@@ -689,7 +697,7 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C11" s="2">
         <v>3</v>
@@ -703,7 +711,7 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C12" s="2">
         <v>4</v>
@@ -722,8 +730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,6 +818,9 @@
       <c r="B5" t="s">
         <v>22</v>
       </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
       <c r="D5">
         <v>1995</v>
       </c>
@@ -822,10 +833,10 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D6">
         <v>1936</v>
@@ -839,13 +850,13 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D7">
-        <v>2025</v>
+        <v>2003</v>
       </c>
       <c r="E7" t="s">
         <v>16</v>
@@ -856,10 +867,10 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D8">
         <v>1989</v>

</xml_diff>